<commit_message>
falta as rules, e ver se queremos imagens nos slides
</commit_message>
<xml_diff>
--- a/Parte_2/Parte_2_Excel.xlsx
+++ b/Parte_2/Parte_2_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c679ef514fe8a1b6/Área de Trabalho/SI_2_TP/Parte_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="865" documentId="13_ncr:1_{8A4C9C23-7A8E-4081-BB61-A08E41E0879A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0C36ED9-52D7-4A7C-81B7-ECBE49E2A412}"/>
+  <xr:revisionPtr revIDLastSave="975" documentId="13_ncr:1_{8A4C9C23-7A8E-4081-BB61-A08E41E0879A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A61E401-C1DB-4E34-9240-2CED98362C34}"/>
   <bookViews>
     <workbookView xWindow="1410" yWindow="0" windowWidth="25800" windowHeight="11385" activeTab="1" xr2:uid="{697C5C7C-CF60-4D59-8825-FC3BC12B99DE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="54">
   <si>
     <t>Descision Tree</t>
   </si>
@@ -192,10 +192,13 @@
     <t>Cluster Count 3</t>
   </si>
   <si>
-    <t>Cluster Count 10</t>
-  </si>
-  <si>
     <t>0,88</t>
+  </si>
+  <si>
+    <t>0,86</t>
+  </si>
+  <si>
+    <t>Cluster Count 20</t>
   </si>
 </sst>
 </file>
@@ -304,7 +307,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -320,6 +323,8 @@
     <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,9 +334,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -656,7 +658,7 @@
   <dimension ref="A2:W57"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,26 +679,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="N2" s="10" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="N2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -2890,7 +2892,7 @@
         <v>47</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
         <v>33</v>
@@ -3025,10 +3027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92C9654-A3AF-4BC5-A51F-5650056B6E18}">
-  <dimension ref="A2:W57"/>
+  <dimension ref="A2:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,7 +3039,7 @@
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="7" max="8" width="11.140625" style="12" customWidth="1"/>
+    <col min="7" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="12" max="13" width="9.140625" style="2"/>
@@ -3049,26 +3051,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="N2" s="10" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="N2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -3260,8 +3262,8 @@
       <c r="F7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="6" t="s">
         <v>33</v>
       </c>
@@ -3516,8 +3518,8 @@
       <c r="F14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
       <c r="I14" s="7" t="s">
         <v>33</v>
       </c>
@@ -3694,8 +3696,8 @@
       <c r="F19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="7" t="s">
         <v>33</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>19</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M21" s="2">
         <f>(6004 + 1155)/(6004 + 1155 + 1057 + 832)</f>
@@ -3868,8 +3870,8 @@
       <c r="F24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="7" t="s">
         <v>33</v>
       </c>
@@ -4046,8 +4048,8 @@
       <c r="F29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="7" t="s">
         <v>19</v>
       </c>
@@ -4315,310 +4317,431 @@
         <v>0.88703650474274209</v>
       </c>
     </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="7"/>
+      <c r="L36" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M36" s="8">
+        <f>(6237 + 1251)/(6237 + 1251 + 599 + 961)</f>
+        <v>0.82758620689655171</v>
+      </c>
+      <c r="N36" s="8">
+        <f>(1251)/(1251 + 599)</f>
+        <v>0.67621621621621619</v>
+      </c>
+      <c r="O36" s="8">
+        <f>(1251)/(1251 + 961)</f>
+        <v>0.56555153707052441</v>
+      </c>
+      <c r="P36" s="8">
+        <f>2*M36*O36/(M36 + O36)</f>
+        <v>0.6719258786800496</v>
+      </c>
+      <c r="Q36" s="8">
+        <f>(6237)/(6237 + 961)</f>
+        <v>0.86649069185884964</v>
+      </c>
+      <c r="R36" s="8">
+        <f>(6237)/(6237 + 599)</f>
+        <v>0.91237565827969569</v>
+      </c>
+      <c r="S36" s="8">
+        <f>2*Q36*R36/(Q36+R36)</f>
+        <v>0.88884138520735356</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M38" s="2">
+        <f>(6158 + 1327)/(6158 + 1327 + 678 + 885)</f>
+        <v>0.82725464190981435</v>
+      </c>
+      <c r="N38" s="2">
+        <f>(1327)/(1327 + 678)</f>
+        <v>0.66184538653366587</v>
+      </c>
+      <c r="O38" s="2">
+        <f>(1327)/(1327 + 885)</f>
+        <v>0.59990958408679929</v>
+      </c>
+      <c r="P38" s="2">
+        <f>2*M38*O38/(M38 + O38)</f>
+        <v>0.69547425464007995</v>
+      </c>
+      <c r="Q38" s="2">
+        <f>(6158)/(6158 + 885)</f>
+        <v>0.87434331960812151</v>
+      </c>
+      <c r="R38" s="2">
+        <f>(6158)/(6158 + 678)</f>
+        <v>0.9008191925102399</v>
+      </c>
+      <c r="S38" s="2">
+        <f>2*Q38*R38/(Q38+R38)</f>
+        <v>0.88738381727790183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J39" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="2">
+        <f>(6178 + 1304)/(6178 + 1304 + 658 + 908)</f>
+        <v>0.82692307692307687</v>
+      </c>
+      <c r="N39" s="2">
+        <f>(1304)/(1304 + 658)</f>
+        <v>0.66462793068297654</v>
+      </c>
+      <c r="O39" s="2">
+        <f>(1304)/(1304 + 908)</f>
+        <v>0.58951175406871614</v>
+      </c>
+      <c r="P39" s="2">
+        <f>2*M39*O39/(M39 + O39)</f>
+        <v>0.68832093491443869</v>
+      </c>
+      <c r="Q39" s="2">
+        <f>(6178)/(6178 + 908)</f>
+        <v>0.87186000564493371</v>
+      </c>
+      <c r="R39" s="2">
+        <f>(6178)/(6178 + 658)</f>
+        <v>0.90374488004681097</v>
+      </c>
+      <c r="S39" s="2">
+        <f>2*Q39*R39/(Q39+R39)</f>
+        <v>0.88751616147105306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s">
-        <v>19</v>
-      </c>
-      <c r="I41" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" t="s">
-        <v>19</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M41" s="2">
-        <f>(6249 + 1522)/(6249 + 1522 + 464 + 813)</f>
-        <v>0.85886383731211313</v>
-      </c>
-      <c r="N41" s="2">
-        <f>(1522)/(1522 + 464)</f>
-        <v>0.76636455186304131</v>
-      </c>
-      <c r="O41" s="2">
-        <f>(1522)/(1522 + 813)</f>
-        <v>0.65182012847965742</v>
-      </c>
-      <c r="P41" s="2">
-        <f>2*N41*O41/(N41 + O41)</f>
-        <v>0.70446655866697527</v>
-      </c>
-      <c r="Q41" s="2">
-        <f>(6249)/(6249 + 813)</f>
-        <v>0.88487680543755309</v>
-      </c>
-      <c r="R41" s="2">
-        <f>(6249)/(6249 + 464)</f>
-        <v>0.93088038134962015</v>
-      </c>
-      <c r="S41" s="2">
-        <f>2*Q41*R41/(Q41 + R41)</f>
-        <v>0.90729582577132484</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" t="s">
-        <v>19</v>
-      </c>
-      <c r="I42" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M42" s="2">
-        <f>(6252 + 1527)/(6252 + 1527 + 461 + 808)</f>
-        <v>0.85974801061007955</v>
-      </c>
-      <c r="N42" s="2">
-        <f>(1527)/(1527 + 461)</f>
-        <v>0.76810865191146882</v>
-      </c>
-      <c r="O42" s="2">
-        <f>(1527)/(1527 + 808)</f>
-        <v>0.65396145610278378</v>
-      </c>
-      <c r="P42" s="2">
-        <f>2*N42*O42/(N42 + O42)</f>
-        <v>0.70645385149201956</v>
-      </c>
-      <c r="Q42" s="2">
-        <f>(6252)/(6252 + 808)</f>
-        <v>0.88555240793201129</v>
-      </c>
-      <c r="R42" s="2">
-        <f>(6252)/(6252 + 461)</f>
-        <v>0.93132727543572169</v>
-      </c>
-      <c r="S42" s="2">
-        <f>2*Q42*R42/(Q42 + R42)</f>
-        <v>0.90786321062949249</v>
+      <c r="C41" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" s="7"/>
+      <c r="L41" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M41" s="8">
+        <f>(6178 + 1304)/(6178 + 1304 + 658 + 908)</f>
+        <v>0.82692307692307687</v>
+      </c>
+      <c r="N41" s="8">
+        <f>(1304)/(1304 + 658)</f>
+        <v>0.66462793068297654</v>
+      </c>
+      <c r="O41" s="8">
+        <f>(1304)/(1304 + 908)</f>
+        <v>0.58951175406871614</v>
+      </c>
+      <c r="P41" s="8">
+        <f>2*M41*O41/(M41 + O41)</f>
+        <v>0.68832093491443869</v>
+      </c>
+      <c r="Q41" s="8">
+        <f>(6178)/(6178 + 908)</f>
+        <v>0.87186000564493371</v>
+      </c>
+      <c r="R41" s="8">
+        <f>(6178)/(6178 + 658)</f>
+        <v>0.90374488004681097</v>
+      </c>
+      <c r="S41" s="8">
+        <f>2*Q41*R41/(Q41+R41)</f>
+        <v>0.88751616147105306</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
       </c>
-      <c r="C43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" t="s">
-        <v>19</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M43" s="2">
-        <f>(6212 + 1441)/(6212 + 1441 + 501 + 894)</f>
-        <v>0.84582228116710878</v>
-      </c>
-      <c r="N43" s="2">
-        <f>(1441)/(1441 + 501)</f>
-        <v>0.74201853759011327</v>
-      </c>
-      <c r="O43" s="2">
-        <f>(1441)/(1441 + 894)</f>
-        <v>0.6171306209850107</v>
-      </c>
-      <c r="P43" s="2">
-        <f>2*N43*O43/(N43 + O43)</f>
-        <v>0.67383680149637593</v>
-      </c>
-      <c r="Q43" s="2">
-        <f>(6212)/(6212 + 894)</f>
-        <v>0.87419082465522091</v>
-      </c>
-      <c r="R43" s="2">
-        <f>(6212)/(6212 + 501)</f>
-        <v>0.92536868762103386</v>
-      </c>
-      <c r="S43" s="2">
-        <f>2*Q43*R43/(Q43 + R43)</f>
-        <v>0.89905202981402421</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>19</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J44" t="s">
-        <v>19</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M44" s="2">
-        <f>(6196 + 1471)/(6196 + 1471 + 517 + 864)</f>
-        <v>0.84736958443854993</v>
-      </c>
-      <c r="N44" s="2">
-        <f>(1471)/(1471 + 517)</f>
-        <v>0.73993963782696182</v>
-      </c>
-      <c r="O44" s="2">
-        <f>(1471)/(1471 + 864)</f>
-        <v>0.62997858672376872</v>
-      </c>
-      <c r="P44" s="2">
-        <f>2*N44*O44/(N44 + O44)</f>
-        <v>0.68054591718713853</v>
-      </c>
-      <c r="Q44" s="2">
-        <f>(6196)/(6196 + 864)</f>
-        <v>0.87762039660056657</v>
-      </c>
-      <c r="R44" s="2">
-        <f>(6196)/(6196 + 517)</f>
-        <v>0.92298525249515861</v>
-      </c>
-      <c r="S44" s="2">
-        <f>2*Q44*R44/(Q44 + R44)</f>
-        <v>0.899731358454948</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M46" s="8">
-        <f>(6252 + 1527)/(6252 + 1527 + 461 + 808)</f>
-        <v>0.85974801061007955</v>
-      </c>
-      <c r="N46" s="8">
-        <f>(1527)/(1527 + 461)</f>
-        <v>0.76810865191146882</v>
-      </c>
-      <c r="O46" s="8">
-        <f>(1527)/(1527 + 808)</f>
-        <v>0.65396145610278378</v>
-      </c>
-      <c r="P46" s="8">
-        <f>2*N46*O46/(N46 + O46)</f>
-        <v>0.70645385149201956</v>
-      </c>
-      <c r="Q46" s="8">
-        <f>(6252)/(6252 + 808)</f>
-        <v>0.88555240793201129</v>
-      </c>
-      <c r="R46" s="8">
-        <f>(6252)/(6252 + 461)</f>
-        <v>0.93132727543572169</v>
-      </c>
-      <c r="S46" s="8">
-        <f>2*Q46*R46/(Q46 + R46)</f>
-        <v>0.90786321062949249</v>
-      </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>46</v>
+      <c r="A48" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
       </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M48" s="2">
+        <f>(6254 + 1196)/(6254 + 1196 + 582 + 1017)</f>
+        <v>0.82329539175599509</v>
+      </c>
+      <c r="N48" s="2">
+        <f>(1196)/(1196 + 582)</f>
+        <v>0.67266591676040499</v>
+      </c>
+      <c r="O48" s="2">
+        <f>(1196)/(1196 + 1017)</f>
+        <v>0.5404428377767736</v>
+      </c>
+      <c r="P48" s="2">
+        <f>2*M48*O48/(M48 + O48)</f>
+        <v>0.65253593132986099</v>
+      </c>
+      <c r="Q48" s="2">
+        <f>(6254)/(6254 + 1017)</f>
+        <v>0.86012928070416728</v>
+      </c>
+      <c r="R48" s="2">
+        <f>(6254)/(6254 + 582)</f>
+        <v>0.91486249268578113</v>
+      </c>
+      <c r="S48" s="2">
+        <f>2*Q48*R48/(Q48+R48)</f>
+        <v>0.88665201672928329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M49" s="2">
+        <f>(6314 + 969)/(6314 + 969 + 522 + 1243)</f>
+        <v>0.80492926613616267</v>
+      </c>
+      <c r="N49" s="2">
+        <f>(969)/(969 + 522)</f>
+        <v>0.64989939637826966</v>
+      </c>
+      <c r="O49" s="2">
+        <f>(969)/(969 + 1243)</f>
+        <v>0.43806509945750455</v>
+      </c>
+      <c r="P49" s="2">
+        <f>2*M49*O49/(M49 + O49)</f>
+        <v>0.5673580328061798</v>
+      </c>
+      <c r="Q49" s="2">
+        <f>(6314)/(6314 + 1243)</f>
+        <v>0.83551673944687044</v>
+      </c>
+      <c r="R49" s="2">
+        <f>(6314)/(6314 + 522)</f>
+        <v>0.92363955529549446</v>
+      </c>
+      <c r="S49" s="2">
+        <f>2*Q49*R49/(Q49+R49)</f>
+        <v>0.87737094420899042</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J50" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M50" s="2">
+        <f>(6456 + 638)/(6456 + 638 + 1574 + 380)</f>
+        <v>0.78404067197170646</v>
+      </c>
+      <c r="N50" s="2">
+        <f>(638)/(638 + 380)</f>
+        <v>0.62671905697445973</v>
+      </c>
+      <c r="O50" s="2">
+        <f>(638)/(638 + 1574)</f>
+        <v>0.2884267631103074</v>
+      </c>
+      <c r="P50" s="2">
+        <f>2*M50*O50/(M50 + O50)</f>
+        <v>0.42171595288827834</v>
+      </c>
+      <c r="Q50" s="2">
+        <f>(6456)/(6456 + 1574)</f>
+        <v>0.8039850560398506</v>
+      </c>
+      <c r="R50" s="2">
+        <f>(6456)/(6456 + 380)</f>
+        <v>0.94441193680514923</v>
+      </c>
+      <c r="S50" s="2">
+        <f>2*Q50*R50/(Q50+R50)</f>
+        <v>0.86855912821202752</v>
+      </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B51" t="s">
-        <v>1</v>
+      <c r="B51" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C51" t="s">
         <v>33</v>
@@ -4642,322 +4765,149 @@
         <v>42</v>
       </c>
       <c r="M51" s="2">
-        <f>(6523 + 596)/(6523 + 596 + 190 + 1739)</f>
-        <v>0.7868037135278515</v>
-      </c>
-      <c r="N51" s="2">
-        <f>(596)/(596 + 190)</f>
-        <v>0.75826972010178118</v>
+        <f>(6836 + 0)/(6836 + 0 + 0 + 2212)</f>
+        <v>0.75552608311228997</v>
+      </c>
+      <c r="N51" s="2" t="e">
+        <f>(0)/(0 + 0)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="O51" s="2">
-        <f>(596)/(596 + 1739)</f>
-        <v>0.25524625267665951</v>
+        <f>(0)/(0 + 2212)</f>
+        <v>0</v>
       </c>
       <c r="P51" s="2">
-        <f>2*N51*O51/(N51 + O51)</f>
-        <v>0.38192886895225886</v>
+        <f>2*M51*O51/(M51 + O51)</f>
+        <v>0</v>
       </c>
       <c r="Q51" s="2">
-        <f>(6523)/(6523+ 1739)</f>
-        <v>0.78951827644638106</v>
+        <f>(6836)/(6836 + 2212)</f>
+        <v>0.75552608311228997</v>
       </c>
       <c r="R51" s="2">
-        <f>(6523)/(6523 + 190)</f>
-        <v>0.97169670788023244</v>
+        <f>(6836)/(6836 + 0)</f>
+        <v>1</v>
       </c>
       <c r="S51" s="2">
-        <f>2*Q51*R51/(Q51 + R51)</f>
-        <v>0.87118530884808021</v>
+        <f>2*Q51*R51/(Q51+R51)</f>
+        <v>0.86074036766557538</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J52" t="s">
+        <v>19</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M52" s="2">
+        <f>(6297 + 943)/(6297 + 943 + 539 + 1269)</f>
+        <v>0.80017683465959333</v>
+      </c>
+      <c r="N52" s="2">
+        <f>(943)/(943 + 539)</f>
+        <v>0.63630229419703099</v>
+      </c>
+      <c r="O52" s="2">
+        <f>(943)/(943 + 1269)</f>
+        <v>0.42631103074141047</v>
+      </c>
+      <c r="P52" s="2">
+        <f>2*M52*O52/(M52 + O52)</f>
+        <v>0.55626186085028861</v>
+      </c>
+      <c r="Q52" s="2">
+        <f>(6297)/(6297 + 1269)</f>
+        <v>0.83227597145122922</v>
+      </c>
+      <c r="R52" s="2">
+        <f>(6297)/(6297 + 539)</f>
+        <v>0.92115272088940903</v>
+      </c>
+      <c r="S52" s="2">
+        <f>2*Q52*R52/(Q52+R52)</f>
+        <v>0.87446188029440364</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C52" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" t="s">
-        <v>33</v>
-      </c>
-      <c r="J52" t="s">
-        <v>19</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M52" s="2">
-        <f>(6443 + 670)/(6443 + 670 + 270 + 1665)</f>
-        <v>0.78614058355437666</v>
-      </c>
-      <c r="N52" s="2">
-        <f>(670)/(670 + 270)</f>
-        <v>0.71276595744680848</v>
-      </c>
-      <c r="O52" s="2">
-        <f>(670)/(670 + 1665)</f>
-        <v>0.28693790149892934</v>
-      </c>
-      <c r="P52" s="2">
-        <f>2*N52*O52/(N52 + O52)</f>
-        <v>0.40916030534351144</v>
-      </c>
-      <c r="Q52" s="2">
-        <f>(6443)/(6443 + 1665)</f>
-        <v>0.79464726196349289</v>
-      </c>
-      <c r="R52" s="2">
-        <f>(6443)/(6443 + 270)</f>
-        <v>0.95977953225085655</v>
-      </c>
-      <c r="S52" s="2">
-        <f>2*Q52*R52/(Q52 + R52)</f>
-        <v>0.86944200796167603</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
-        <v>19</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J53" t="s">
-        <v>19</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M53" s="2">
-        <f>(6547 + 576)/(6547 + 576 + 1759 + 166)</f>
-        <v>0.78724580017683465</v>
-      </c>
-      <c r="N53" s="2">
-        <f>(576)/(576 + 166)</f>
-        <v>0.77628032345013476</v>
-      </c>
-      <c r="O53" s="2">
-        <f>(576)/(576 + 1759)</f>
-        <v>0.24668094218415418</v>
-      </c>
-      <c r="P53" s="2">
-        <f>2*N53*O53/(N53 + O53)</f>
-        <v>0.37439064023399415</v>
-      </c>
-      <c r="Q53" s="2">
-        <f>(6547)/(6547+ 1759)</f>
-        <v>0.78822537924392011</v>
-      </c>
-      <c r="R53" s="2">
-        <f>(6547)/(6547 + 166)</f>
-        <v>0.97527186056904513</v>
-      </c>
-      <c r="S53" s="2">
-        <f>2*Q53*R53/(Q53 + R53)</f>
-        <v>0.87182901657900003</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
-        <v>19</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J54" t="s">
-        <v>19</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M54" s="2">
-        <f>(6096 + 1068)/(6096 + 1068 + 1267 + 617)</f>
-        <v>0.79177718832891242</v>
-      </c>
-      <c r="N54" s="2">
-        <f>(1068)/(1068 + 617)</f>
-        <v>0.63382789317507415</v>
-      </c>
-      <c r="O54" s="2">
-        <f>(1068)/(1068 + 1267)</f>
-        <v>0.45738758029978588</v>
-      </c>
-      <c r="P54" s="2">
-        <f>2*N54*O54/(N54 + O54)</f>
-        <v>0.53134328358208949</v>
-      </c>
-      <c r="Q54" s="2">
-        <f>(6096)/(6096 + 1267)</f>
-        <v>0.82792340078772242</v>
-      </c>
-      <c r="R54" s="2">
-        <f>(6096)/(6096 + 617)</f>
-        <v>0.90808878295843887</v>
-      </c>
-      <c r="S54" s="2">
-        <f>2*Q54*R54/(Q54 + R54)</f>
-        <v>0.86615515771526008</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" t="s">
-        <v>19</v>
-      </c>
-      <c r="E55" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" t="s">
-        <v>19</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M55" s="2">
-        <f>(6232 + 1089)/(6232 + 1089 + 481 + 1246)</f>
-        <v>0.80912908930150307</v>
-      </c>
-      <c r="N55" s="2">
-        <f>(1089)/(1089 + 481)</f>
-        <v>0.6936305732484076</v>
-      </c>
-      <c r="O55" s="2">
-        <f>(1089)/(1089 + 1246)</f>
-        <v>0.46638115631691651</v>
-      </c>
-      <c r="P55" s="2">
-        <f>2*N55*O55/(N55 + O55)</f>
-        <v>0.55774647887323947</v>
-      </c>
-      <c r="Q55" s="2">
-        <f>(6232)/(6232 + 1246)</f>
-        <v>0.83337790853169291</v>
-      </c>
-      <c r="R55" s="2">
-        <f>(6232)/(6232 + 481)</f>
-        <v>0.92834798152837772</v>
-      </c>
-      <c r="S55" s="2">
-        <f>2*Q55*R55/(Q55 + R55)</f>
-        <v>0.87830314988372904</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K57" s="7"/>
-      <c r="L57" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="M57" s="8">
-        <f>(6547 + 576)/(6547 + 576 + 1759 + 166)</f>
-        <v>0.78724580017683465</v>
-      </c>
-      <c r="N57" s="8">
-        <f>(576)/(576 + 166)</f>
-        <v>0.77628032345013476</v>
-      </c>
-      <c r="O57" s="8">
-        <f>(576)/(576 + 1759)</f>
-        <v>0.24668094218415418</v>
-      </c>
-      <c r="P57" s="8">
-        <f>2*N57*O57/(N57 + O57)</f>
-        <v>0.37439064023399415</v>
-      </c>
-      <c r="Q57" s="8">
-        <f>(6547)/(6547+ 1759)</f>
-        <v>0.78822537924392011</v>
-      </c>
-      <c r="R57" s="8">
-        <f>(6547)/(6547 + 166)</f>
-        <v>0.97527186056904513</v>
-      </c>
-      <c r="S57" s="8">
-        <f>2*Q57*R57/(Q57 + R57)</f>
-        <v>0.87182901657900003</v>
+      <c r="C54" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="7"/>
+      <c r="L54" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M54" s="8">
+        <f>(6254 + 1196)/(6254 + 1196 + 582 + 1017)</f>
+        <v>0.82329539175599509</v>
+      </c>
+      <c r="N54" s="8">
+        <f>(1196)/(1196 + 582)</f>
+        <v>0.67266591676040499</v>
+      </c>
+      <c r="O54" s="8">
+        <f>(1196)/(1196 + 1017)</f>
+        <v>0.5404428377767736</v>
+      </c>
+      <c r="P54" s="8">
+        <f>2*M54*O54/(M54 + O54)</f>
+        <v>0.65253593132986099</v>
+      </c>
+      <c r="Q54" s="8">
+        <f>(6254)/(6254 + 1017)</f>
+        <v>0.86012928070416728</v>
+      </c>
+      <c r="R54" s="8">
+        <f>(6254)/(6254 + 582)</f>
+        <v>0.91486249268578113</v>
+      </c>
+      <c r="S54" s="8">
+        <f>2*Q54*R54/(Q54+R54)</f>
+        <v>0.88665201672928329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
penso que vou dar como terminado
</commit_message>
<xml_diff>
--- a/Parte_2/Parte_2_Excel.xlsx
+++ b/Parte_2/Parte_2_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c679ef514fe8a1b6/Área de Trabalho/SI_2_TP/Parte_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="975" documentId="13_ncr:1_{8A4C9C23-7A8E-4081-BB61-A08E41E0879A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A61E401-C1DB-4E34-9240-2CED98362C34}"/>
+  <xr:revisionPtr revIDLastSave="1074" documentId="13_ncr:1_{8A4C9C23-7A8E-4081-BB61-A08E41E0879A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B07E7C03-A3B2-4B8A-B79C-CEEF88DFD7AE}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="0" windowWidth="25800" windowHeight="11385" activeTab="1" xr2:uid="{697C5C7C-CF60-4D59-8825-FC3BC12B99DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{697C5C7C-CF60-4D59-8825-FC3BC12B99DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sugested" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="54">
   <si>
     <t>Descision Tree</t>
   </si>
@@ -655,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431C9455-E997-42FE-9C36-1F409FB01350}">
-  <dimension ref="A2:W57"/>
+  <dimension ref="A2:W59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,16 +2628,197 @@
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
       </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="M48" s="2">
+        <f>(6611 + 618)/(6611 + 618 + 1717 + 102)</f>
+        <v>0.79896109637488943</v>
+      </c>
+      <c r="N48" s="2">
+        <f>(618)/(618 + 102)</f>
+        <v>0.85833333333333328</v>
+      </c>
+      <c r="O48" s="2">
+        <f>(618)/(618 + 1717)</f>
+        <v>0.26466809421841542</v>
+      </c>
+      <c r="P48" s="2">
+        <f>2*N48*O48/(N48 + O48)</f>
+        <v>0.40458265139116206</v>
+      </c>
+      <c r="Q48" s="2">
+        <f>(6611)/(6611 + 1717)</f>
+        <v>0.79382804995196921</v>
+      </c>
+      <c r="R48" s="2">
+        <f>(6611)/(6611 + 102)</f>
+        <v>0.98480560107254578</v>
+      </c>
+      <c r="S48" s="2">
+        <f>2*Q48*R48/(Q48 + R48)</f>
+        <v>0.87906389202845547</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" t="s">
+        <v>19</v>
+      </c>
+      <c r="H49" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="M49" s="2">
+        <f>(6612 + 852)/(6612 + 852 + 101 + 1483)</f>
+        <v>0.82493368700265257</v>
+      </c>
+      <c r="N49" s="2">
+        <f>(852)/(852 + 101)</f>
+        <v>0.8940188877229801</v>
+      </c>
+      <c r="O49" s="2">
+        <f>(852)/(852 + 1483)</f>
+        <v>0.36488222698072803</v>
+      </c>
+      <c r="P49" s="2">
+        <f>2*N49*O49/(N49 + O49)</f>
+        <v>0.51824817518248179</v>
+      </c>
+      <c r="Q49" s="2">
+        <f>(6612)/(6612 + 1483)</f>
+        <v>0.81680049413218037</v>
+      </c>
+      <c r="R49" s="2">
+        <f>(6612)/(6612 + 101)</f>
+        <v>0.98495456576791296</v>
+      </c>
+      <c r="S49" s="2">
+        <f>2*Q49*R49/(Q49 + R49)</f>
+        <v>0.89303079416531594</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I50" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="M50" s="2">
+        <f>(6552 + 825)/(6552 + 825 + 161 + 1510)</f>
+        <v>0.81531830238726788</v>
+      </c>
+      <c r="N50" s="2">
+        <f>(825)/(825 + 161)</f>
+        <v>0.83671399594320484</v>
+      </c>
+      <c r="O50" s="2">
+        <f>(825)/(825 + 1510)</f>
+        <v>0.35331905781584583</v>
+      </c>
+      <c r="P50" s="2">
+        <f>2*N50*O50/(N50 + O50)</f>
+        <v>0.49683830171635052</v>
+      </c>
+      <c r="Q50" s="2">
+        <f>(6552)/(6552 + 1510)</f>
+        <v>0.81270156288762097</v>
+      </c>
+      <c r="R50" s="2">
+        <f>(6552)/(6552 + 161)</f>
+        <v>0.97601668404588116</v>
+      </c>
+      <c r="S50" s="2">
+        <f>2*Q50*R50/(Q50 + R50)</f>
+        <v>0.88690355329949244</v>
+      </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>47</v>
+      <c r="A51" t="s">
+        <v>46</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -2655,236 +2836,173 @@
         <v>19</v>
       </c>
       <c r="G51" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H51" t="s">
-        <v>19</v>
-      </c>
-      <c r="I51" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J51" t="s">
         <v>19</v>
       </c>
-      <c r="L51" s="2" t="s">
+      <c r="L51" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="M51" s="2">
+        <f>(6548 + 828)/(6548 + 828 + 1507 + 165)</f>
+        <v>0.81520778072502209</v>
+      </c>
+      <c r="N51" s="2">
+        <f>(828)/( 828 + 165)</f>
+        <v>0.83383685800604235</v>
+      </c>
+      <c r="O51" s="2">
+        <f>(828)/(828 + 1507)</f>
+        <v>0.35460385438972164</v>
+      </c>
+      <c r="P51" s="2">
+        <f>2*N51*O51/(N51 + O51)</f>
+        <v>0.4975961538461538</v>
+      </c>
+      <c r="Q51" s="2">
+        <f>(6548)/(6548 + 1665)</f>
+        <v>0.79727261658346527</v>
+      </c>
+      <c r="R51" s="2">
+        <f>(6548)/(6548+ 165)</f>
+        <v>0.97542082526441232</v>
+      </c>
+      <c r="S51" s="2">
+        <f>2*Q51*R51/(Q51 + R51)</f>
+        <v>0.87739514940372498</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" t="s">
+        <v>19</v>
+      </c>
+      <c r="H53" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J53" t="s">
+        <v>19</v>
+      </c>
+      <c r="L53" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M51" s="2">
+      <c r="M53" s="2">
         <f>(6523 + 596)/(6523 + 596 + 190 + 1739)</f>
         <v>0.7868037135278515</v>
       </c>
-      <c r="N51" s="2">
+      <c r="N53" s="2">
         <f>(596)/(596 + 190)</f>
         <v>0.75826972010178118</v>
       </c>
-      <c r="O51" s="2">
+      <c r="O53" s="2">
         <f>(596)/(596 + 1739)</f>
         <v>0.25524625267665951</v>
       </c>
-      <c r="P51" s="2">
-        <f>2*N51*O51/(N51 + O51)</f>
+      <c r="P53" s="2">
+        <f>2*N53*O53/(N53 + O53)</f>
         <v>0.38192886895225886</v>
       </c>
-      <c r="Q51" s="2">
+      <c r="Q53" s="2">
         <f>(6523)/(6523+ 1739)</f>
         <v>0.78951827644638106</v>
       </c>
-      <c r="R51" s="2">
+      <c r="R53" s="2">
         <f>(6523)/(6523 + 190)</f>
         <v>0.97169670788023244</v>
       </c>
-      <c r="S51" s="2">
-        <f>2*Q51*R51/(Q51 + R51)</f>
+      <c r="S53" s="2">
+        <f>2*Q53*R53/(Q53 + R53)</f>
         <v>0.87118530884808021</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>47</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>1</v>
       </c>
-      <c r="C52" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I52" t="s">
-        <v>33</v>
-      </c>
-      <c r="J52" t="s">
-        <v>19</v>
-      </c>
-      <c r="L52" s="2" t="s">
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J54" t="s">
+        <v>19</v>
+      </c>
+      <c r="L54" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M52" s="2">
+      <c r="M54" s="2">
         <f>(6443 + 670)/(6443 + 670 + 270 + 1665)</f>
         <v>0.78614058355437666</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N54" s="2">
         <f>(670)/(670 + 270)</f>
         <v>0.71276595744680848</v>
       </c>
-      <c r="O52" s="2">
+      <c r="O54" s="2">
         <f>(670)/(670 + 1665)</f>
         <v>0.28693790149892934</v>
       </c>
-      <c r="P52" s="2">
-        <f>2*N52*O52/(N52 + O52)</f>
+      <c r="P54" s="2">
+        <f>2*N54*O54/(N54 + O54)</f>
         <v>0.40916030534351144</v>
       </c>
-      <c r="Q52" s="2">
+      <c r="Q54" s="2">
         <f>(6443)/(6443 + 1665)</f>
         <v>0.79464726196349289</v>
       </c>
-      <c r="R52" s="2">
+      <c r="R54" s="2">
         <f>(6443)/(6443 + 270)</f>
         <v>0.95977953225085655</v>
       </c>
-      <c r="S52" s="2">
-        <f>2*Q52*R52/(Q52 + R52)</f>
-        <v>0.86944200796167603</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" t="s">
-        <v>19</v>
-      </c>
-      <c r="H53" t="s">
-        <v>19</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J53" t="s">
-        <v>19</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M53" s="2">
-        <f>(6547 + 576)/(6547 + 576 + 1759 + 166)</f>
-        <v>0.78724580017683465</v>
-      </c>
-      <c r="N53" s="2">
-        <f>(576)/(576 + 166)</f>
-        <v>0.77628032345013476</v>
-      </c>
-      <c r="O53" s="2">
-        <f>(576)/(576 + 1759)</f>
-        <v>0.24668094218415418</v>
-      </c>
-      <c r="P53" s="2">
-        <f>2*N53*O53/(N53 + O53)</f>
-        <v>0.37439064023399415</v>
-      </c>
-      <c r="Q53" s="2">
-        <f>(6547)/(6547+ 1759)</f>
-        <v>0.78822537924392011</v>
-      </c>
-      <c r="R53" s="2">
-        <f>(6547)/(6547 + 166)</f>
-        <v>0.97527186056904513</v>
-      </c>
-      <c r="S53" s="2">
-        <f>2*Q53*R53/(Q53 + R53)</f>
-        <v>0.87182901657900003</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54" t="s">
-        <v>19</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J54" t="s">
-        <v>19</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M54" s="2">
-        <f>(6096 + 1068)/(6096 + 1068 + 1267 + 617)</f>
-        <v>0.79177718832891242</v>
-      </c>
-      <c r="N54" s="2">
-        <f>(1068)/(1068 + 617)</f>
-        <v>0.63382789317507415</v>
-      </c>
-      <c r="O54" s="2">
-        <f>(1068)/(1068 + 1267)</f>
-        <v>0.45738758029978588</v>
-      </c>
-      <c r="P54" s="2">
-        <f>2*N54*O54/(N54 + O54)</f>
-        <v>0.53134328358208949</v>
-      </c>
-      <c r="Q54" s="2">
-        <f>(6096)/(6096 + 1267)</f>
-        <v>0.82792340078772242</v>
-      </c>
-      <c r="R54" s="2">
-        <f>(6096)/(6096 + 617)</f>
-        <v>0.90808878295843887</v>
-      </c>
       <c r="S54" s="2">
         <f>2*Q54*R54/(Q54 + R54)</f>
-        <v>0.86615515771526008</v>
+        <v>0.86944200796167603</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
@@ -2892,125 +3010,251 @@
         <v>47</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" t="s">
+        <v>19</v>
+      </c>
+      <c r="H55" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" t="s">
+        <v>19</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M55" s="2">
+        <f>(6547 + 576)/(6547 + 576 + 1759 + 166)</f>
+        <v>0.78724580017683465</v>
+      </c>
+      <c r="N55" s="2">
+        <f>(576)/(576 + 166)</f>
+        <v>0.77628032345013476</v>
+      </c>
+      <c r="O55" s="2">
+        <f>(576)/(576 + 1759)</f>
+        <v>0.24668094218415418</v>
+      </c>
+      <c r="P55" s="2">
+        <f>2*N55*O55/(N55 + O55)</f>
+        <v>0.37439064023399415</v>
+      </c>
+      <c r="Q55" s="2">
+        <f>(6547)/(6547+ 1759)</f>
+        <v>0.78822537924392011</v>
+      </c>
+      <c r="R55" s="2">
+        <f>(6547)/(6547 + 166)</f>
+        <v>0.97527186056904513</v>
+      </c>
+      <c r="S55" s="2">
+        <f>2*Q55*R55/(Q55 + R55)</f>
+        <v>0.87182901657900003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" t="s">
+        <v>19</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" t="s">
+        <v>19</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M56" s="2">
+        <f>(6096 + 1068)/(6096 + 1068 + 1267 + 617)</f>
+        <v>0.79177718832891242</v>
+      </c>
+      <c r="N56" s="2">
+        <f>(1068)/(1068 + 617)</f>
+        <v>0.63382789317507415</v>
+      </c>
+      <c r="O56" s="2">
+        <f>(1068)/(1068 + 1267)</f>
+        <v>0.45738758029978588</v>
+      </c>
+      <c r="P56" s="2">
+        <f>2*N56*O56/(N56 + O56)</f>
+        <v>0.53134328358208949</v>
+      </c>
+      <c r="Q56" s="2">
+        <f>(6096)/(6096 + 1267)</f>
+        <v>0.82792340078772242</v>
+      </c>
+      <c r="R56" s="2">
+        <f>(6096)/(6096 + 617)</f>
+        <v>0.90808878295843887</v>
+      </c>
+      <c r="S56" s="2">
+        <f>2*Q56*R56/(Q56 + R56)</f>
+        <v>0.86615515771526008</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C55" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" t="s">
-        <v>19</v>
-      </c>
-      <c r="E55" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" t="s">
-        <v>19</v>
-      </c>
-      <c r="H55" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" t="s">
-        <v>19</v>
-      </c>
-      <c r="L55" s="2" t="s">
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" t="s">
+        <v>19</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J57" t="s">
+        <v>19</v>
+      </c>
+      <c r="L57" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M55" s="2">
+      <c r="M57" s="2">
         <f>(6232 + 1089)/(6232 + 1089 + 481 + 1246)</f>
         <v>0.80912908930150307</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N57" s="2">
         <f>(1089)/(1089 + 481)</f>
         <v>0.6936305732484076</v>
       </c>
-      <c r="O55" s="2">
+      <c r="O57" s="2">
         <f>(1089)/(1089 + 1246)</f>
         <v>0.46638115631691651</v>
       </c>
-      <c r="P55" s="2">
-        <f>2*N55*O55/(N55 + O55)</f>
+      <c r="P57" s="2">
+        <f>2*N57*O57/(N57 + O57)</f>
         <v>0.55774647887323947</v>
       </c>
-      <c r="Q55" s="2">
+      <c r="Q57" s="2">
         <f>(6232)/(6232 + 1246)</f>
         <v>0.83337790853169291</v>
       </c>
-      <c r="R55" s="2">
+      <c r="R57" s="2">
         <f>(6232)/(6232 + 481)</f>
         <v>0.92834798152837772</v>
       </c>
-      <c r="S55" s="2">
-        <f>2*Q55*R55/(Q55 + R55)</f>
+      <c r="S57" s="2">
+        <f>2*Q57*R57/(Q57 + R57)</f>
         <v>0.87830314988372904</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I57" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K57" s="7"/>
-      <c r="L57" s="8" t="s">
+      <c r="C59" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K59" s="7"/>
+      <c r="L59" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="M57" s="8">
+      <c r="M59" s="8">
         <f>(6547 + 576)/(6547 + 576 + 1759 + 166)</f>
         <v>0.78724580017683465</v>
       </c>
-      <c r="N57" s="8">
+      <c r="N59" s="8">
         <f>(576)/(576 + 166)</f>
         <v>0.77628032345013476</v>
       </c>
-      <c r="O57" s="8">
+      <c r="O59" s="8">
         <f>(576)/(576 + 1759)</f>
         <v>0.24668094218415418</v>
       </c>
-      <c r="P57" s="8">
-        <f>2*N57*O57/(N57 + O57)</f>
+      <c r="P59" s="8">
+        <f>2*N59*O59/(N59 + O59)</f>
         <v>0.37439064023399415</v>
       </c>
-      <c r="Q57" s="8">
+      <c r="Q59" s="8">
         <f>(6547)/(6547+ 1759)</f>
         <v>0.78822537924392011</v>
       </c>
-      <c r="R57" s="8">
+      <c r="R59" s="8">
         <f>(6547)/(6547 + 166)</f>
         <v>0.97527186056904513</v>
       </c>
-      <c r="S57" s="8">
-        <f>2*Q57*R57/(Q57 + R57)</f>
+      <c r="S59" s="8">
+        <f>2*Q59*R59/(Q59 + R59)</f>
         <v>0.87182901657900003</v>
       </c>
     </row>
@@ -3029,8 +3273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92C9654-A3AF-4BC5-A51F-5650056B6E18}">
   <dimension ref="A2:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4556,11 +4800,117 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="M43" s="2">
+        <f>(6718 + 382)/(6718 + 382 + 118 + 1830)</f>
+        <v>0.7847038019451813</v>
+      </c>
+      <c r="N43" s="2">
+        <f>(382)/(382 + 118)</f>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="O43" s="2">
+        <f>(382)/(382 + 1830)</f>
+        <v>0.17269439421338156</v>
+      </c>
+      <c r="P43" s="2">
+        <f>2*M43*O43/(M43 + O43)</f>
+        <v>0.28308795286557403</v>
+      </c>
+      <c r="Q43" s="2">
+        <f>(6718)/(6718 + 1830)</f>
+        <v>0.78591483387926997</v>
+      </c>
+      <c r="R43" s="2">
+        <f>(6718)/(6718 + 118)</f>
+        <v>0.98273844353423057</v>
+      </c>
+      <c r="S43" s="2">
+        <f>2*Q43*R43/(Q43+R43)</f>
+        <v>0.87337493499739982</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J44" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="M44" s="2">
+        <f>(6721 + 391)/(6721 + 391 + 1821 + 115)</f>
+        <v>0.78603006189213087</v>
+      </c>
+      <c r="N44" s="2">
+        <f>(391)/(391 + 115)</f>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="O44" s="2">
+        <f>(391)/(391 + 1821)</f>
+        <v>0.1767631103074141</v>
+      </c>
+      <c r="P44" s="2">
+        <f>2*M44*O44/(M44 + O44)</f>
+        <v>0.28862090539708529</v>
+      </c>
+      <c r="Q44" s="2">
+        <f>(6721)/(6721 + 1821)</f>
+        <v>0.78681807539217985</v>
+      </c>
+      <c r="R44" s="2">
+        <f>(6721)/(6721+ 115)</f>
+        <v>0.9831772966647162</v>
+      </c>
+      <c r="S44" s="2">
+        <f>2*Q44*R44/(Q44+R44)</f>
+        <v>0.87410586552217451</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>